<commit_message>
Many changes to support 10x CellRanger alignment and QC
</commit_message>
<xml_diff>
--- a/ConfigNotes/autoAnalysis.wf.config.xlsx
+++ b/ConfigNotes/autoAnalysis.wf.config.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0028003/HCI/AutoAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0028003/Code/AutoAnalysis/ConfigNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536A14AB-D701-3A47-B8AA-829D7158014C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA6B82-1EB8-D440-9430-12245106DD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="2200" windowWidth="32160" windowHeight="17440" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
+    <workbookView xWindow="1160" yWindow="1660" windowWidth="32160" windowHeight="17440" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Human</t>
   </si>
@@ -44,39 +44,15 @@
     <t># Organism</t>
   </si>
   <si>
-    <t>D. melanogaster</t>
-  </si>
-  <si>
-    <t>Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection</t>
-  </si>
-  <si>
-    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat)</t>
-  </si>
-  <si>
-    <t>Zebrafish</t>
-  </si>
-  <si>
-    <t>NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation</t>
-  </si>
-  <si>
     <t>Mouse</t>
   </si>
   <si>
-    <t>Marmoset</t>
-  </si>
-  <si>
-    <t>NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat)</t>
-  </si>
-  <si>
     <t># Get Organisms from GNomEx Experiment Overview tab -&gt; Organism</t>
   </si>
   <si>
     <t># Get Library Prep Kits from the  GNomEx Experiment Overview tab -&gt; Library Protocol</t>
   </si>
   <si>
-    <t># Tab delimited AutoAnalysis Organism-LibraryKit : Workflow docs, use exact values from the GNomEx LIMs, case space identical</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -89,10 +65,28 @@
     <t xml:space="preserve">Workflow Paths on RW , comma delimited, files and the contents of provided directories will be copied into each Job dir </t>
   </si>
   <si>
-    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/, /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/human_reverse_truseq_rnaAlignQC.yaml</t>
-  </si>
-  <si>
-    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/, /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/mouse_reverse_truseq_rnaAlignQC.yaml</t>
+    <t>--module cellranger</t>
+  </si>
+  <si>
+    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat)</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/human_reverse_truseq_rnaAlignQC.yaml</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/mouse_reverse_truseq_rnaAlignQC.yaml</t>
+  </si>
+  <si>
+    <t># Tab delimited AutoAnalysis Organism-LibraryKit : Workflow docs, use exact values from the GNomEx LIMs, case space identical, semi-colon delimited within the cell</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Config/mouse_gem_cellRanger.yaml</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Config/human_gem_cellRanger.yaml</t>
+  </si>
+  <si>
+    <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling</t>
   </si>
 </sst>
 </file>
@@ -136,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -162,6 +156,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,39 +474,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1575BC-6DBD-9743-ACB5-EE787B21782E}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="78.83203125" customWidth="1"/>
-    <col min="3" max="3" width="69" style="6" customWidth="1"/>
+    <col min="2" max="3" width="106.6640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="3"/>
     </row>
@@ -518,185 +517,101 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B17">
-    <sortCondition ref="B6:B17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B7">
+    <sortCondition ref="B6:B7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added checker for dnaAlignQC to only launch with R1 and R2 named fastqs.
</commit_message>
<xml_diff>
--- a/ConfigNotes/autoAnalysis.wf.config.xlsx
+++ b/ConfigNotes/autoAnalysis.wf.config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0028003/Code/AutoAnalysis/ConfigNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA6B82-1EB8-D440-9430-12245106DD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E612D0-D9F8-7B46-8D41-D3054BE6EE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1660" windowWidth="32160" windowHeight="17440" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
+    <workbookView xWindow="1920" yWindow="1680" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Human</t>
   </si>
@@ -68,9 +68,6 @@
     <t>--module cellranger</t>
   </si>
   <si>
-    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat)</t>
-  </si>
-  <si>
     <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/human_reverse_truseq_rnaAlignQC.yaml</t>
   </si>
   <si>
@@ -87,13 +84,28 @@
   </si>
   <si>
     <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling</t>
+  </si>
+  <si>
+    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Config/human_novaseq_truseq_dnaAlignQC.yaml</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Config/mouse_novaseq_truseq_dnaAlignQC.yaml</t>
+  </si>
+  <si>
+    <t>Active Motif ATAC-seq; IDT xGEN Human Exome v2 with Nextera Flex Library Prep (1-plex enrichment); IDT xGEN Human Exome v2 with Nextera Flex Library Prep (4-plex enrichment); ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free</t>
+  </si>
+  <si>
+    <t>Active Motif ATAC-seq; ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +120,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -160,6 +178,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,9 +197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +237,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -324,7 +343,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,9 +495,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1575BC-6DBD-9743-ACB5-EE787B21782E}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,7 +509,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -529,15 +548,15 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>5</v>
@@ -548,10 +567,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>5</v>
@@ -565,10 +584,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>9</v>
@@ -579,10 +598,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>9</v>
@@ -591,11 +610,33 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+    <row r="12" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>

</xml_diff>

<commit_message>
Modifications for supporting a yaml config for MultiQC, detailed email debugging when verbose, and adding more info into the Jira tickets.
</commit_message>
<xml_diff>
--- a/ConfigNotes/autoAnalysis.wf.config.xlsx
+++ b/ConfigNotes/autoAnalysis.wf.config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0028003/Code/AutoAnalysis/ConfigNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E612D0-D9F8-7B46-8D41-D3054BE6EE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30777D-7288-1649-8D53-77438914B3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1680" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
+    <workbookView xWindow="-37500" yWindow="3400" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t># Get Library Prep Kits from the  GNomEx Experiment Overview tab -&gt; Library Protocol</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Extra MultiQC Options (e.g. --module cellranger  Or None)</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling</t>
   </si>
   <si>
-    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection</t>
-  </si>
-  <si>
     <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Config/human_novaseq_truseq_dnaAlignQC.yaml</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>Active Motif ATAC-seq; ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free</t>
+  </si>
+  <si>
+    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection; NEBNext Ultra II Directional RNA Library Prep with Globin and rRNA Depletion Kit (human,mouse,rat)</t>
+  </si>
+  <si>
+    <t>--config /home/tomatosrvs/AutoAnalysis/Test/autoAnalysis.multiqc.config.yaml</t>
   </si>
 </sst>
 </file>
@@ -148,15 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -175,10 +172,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,159 +499,162 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="3" width="106.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="58.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="53.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B7">

</xml_diff>

<commit_message>
Adding in output for DRAGEN ORA compression
</commit_message>
<xml_diff>
--- a/ConfigNotes/autoAnalysis.wf.config.xlsx
+++ b/ConfigNotes/autoAnalysis.wf.config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0028003/Code/AutoAnalysis/ConfigNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30777D-7288-1649-8D53-77438914B3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE1533B-8A54-6540-9569-F5D7578C56C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37500" yWindow="3400" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
+    <workbookView xWindow="-48300" yWindow="4840" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Human</t>
   </si>
@@ -74,31 +74,58 @@
     <t># Tab delimited AutoAnalysis Organism-LibraryKit : Workflow docs, use exact values from the GNomEx LIMs, case space identical, semi-colon delimited within the cell</t>
   </si>
   <si>
-    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Config/mouse_gem_cellRanger.yaml</t>
-  </si>
-  <si>
-    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/Config/human_gem_cellRanger.yaml</t>
-  </si>
-  <si>
-    <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling</t>
-  </si>
-  <si>
     <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Config/human_novaseq_truseq_dnaAlignQC.yaml</t>
   </si>
   <si>
     <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Config/mouse_novaseq_truseq_dnaAlignQC.yaml</t>
   </si>
   <si>
-    <t>Active Motif ATAC-seq; IDT xGEN Human Exome v2 with Nextera Flex Library Prep (1-plex enrichment); IDT xGEN Human Exome v2 with Nextera Flex Library Prep (4-plex enrichment); ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free</t>
-  </si>
-  <si>
-    <t>Active Motif ATAC-seq; ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free</t>
-  </si>
-  <si>
-    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection; NEBNext Ultra II Directional RNA Library Prep with Globin and rRNA Depletion Kit (human,mouse,rat)</t>
-  </si>
-  <si>
     <t>--config /home/tomatosrvs/AutoAnalysis/Test/autoAnalysis.multiqc.config.yaml</t>
+  </si>
+  <si>
+    <t>Illumina RNA Exome Library Prep</t>
+  </si>
+  <si>
+    <t>Illumina TruSeq Stranded Total RNA Library Prep Ribo-Zero Gold (Human,Mouse,Rat); NEBNext Ultra II Directional RNA Library Prep with poly(A) mRNA Isolation; NEBNext Ultra II Directional RNA Library Prep with rRNA Depletion Kit (human,mouse,rat); Illumina TruSeq Stranded mRNA Library Preparation Kit with polyA selection; NEBNext Ultra II Directional RNA Library Prep with Globin and rRNA Depletion Kit (human,mouse,rat); Illumina Total RNA Prep with RiboZero Plus</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/RnaAlignQC/AutoAnalysis/Config/human_reverse_nextera_rnaAlignQC.yaml</t>
+  </si>
+  <si>
+    <t>Active Motif ATAC-seq; IDT xGEN Human Exome v2 with Nextera Flex Library Prep (1-plex enrichment); IDT xGEN Human Exome v2 with Nextera Flex Library Prep (4-plex enrichment); ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free; IDT xGEN Human Exome v2 with Nextera Flex Library Prep for FFPE samples (4-plex enrichment); Illumina DNA Prep with UDI</t>
+  </si>
+  <si>
+    <t>Active Motif ATAC-seq; ATAC-seq w/ IDT for Illumina Nextera UD Indexes; ATAC-seq with Nextera XT single index; ChIP-Seq with NEBNext Ultra II DNA Library Prep Kit; Cut&amp;Run with NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit; NEBNext Ultra II DNA Library Prep Kit: PCR-free; IDT xGEN Human Exome v2 with Nextera Flex Library Prep for FFPE samples (4-plex enrichment); Illumina DNA Prep with UDI</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/GEX/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/GEX/Config/mouse_gem_cellRanger.yaml</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/GEX/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/GEX/Config/human_gem_cellRanger.yaml</t>
+  </si>
+  <si>
+    <t># MultiQC doesn't support ATAC so don't set --module cellranger!</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/ATAC/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/ATAC/Config/mouse_atac_cellRanger.yaml</t>
+  </si>
+  <si>
+    <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/ATAC/Run; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/CellRanger/AutoAnalysis/ATAC/Config/human_atac_cellRanger.yaml</t>
+  </si>
+  <si>
+    <t>10x Genomics Chromium Single Cell ATAC Library Preparation, v2</t>
+  </si>
+  <si>
+    <t># 10X</t>
+  </si>
+  <si>
+    <t># Bulk RNASeq</t>
+  </si>
+  <si>
+    <t># DNASeq</t>
+  </si>
+  <si>
+    <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling; 10x Genomics Chromium Next GEM Single Cell  3' Gene Expression Library Preparation v3.1  with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation</t>
   </si>
 </sst>
 </file>
@@ -128,12 +155,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -180,6 +213,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -496,11 +542,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1575BC-6DBD-9743-ACB5-EE787B21782E}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="A1:D13"/>
+      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,112 +595,173 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" s="7" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="7" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="11" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="D12" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
+      <c r="C16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:B7">

</xml_diff>

<commit_message>
Updates to support ORA compression and the move to the hci-dragen server.
</commit_message>
<xml_diff>
--- a/ConfigNotes/autoAnalysis.wf.config.xlsx
+++ b/ConfigNotes/autoAnalysis.wf.config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0028003/Code/AutoAnalysis/ConfigNotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE1533B-8A54-6540-9569-F5D7578C56C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB1EF7-AD86-B448-BF92-48DE57D6FC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48300" yWindow="4840" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="34560" windowHeight="20660" xr2:uid="{8CA74A09-9B93-D44A-8564-7FAFCB43F2A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>/uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Run/; /uufs/chpc.utah.edu/common/PE/hci-bioinformatics1/TNRunner/Workflows/DnaAlignQC/AutoAnalysis/Config/mouse_novaseq_truseq_dnaAlignQC.yaml</t>
   </si>
   <si>
-    <t>--config /home/tomatosrvs/AutoAnalysis/Test/autoAnalysis.multiqc.config.yaml</t>
-  </si>
-  <si>
     <t>Illumina RNA Exome Library Prep</t>
   </si>
   <si>
@@ -125,7 +122,10 @@
     <t># DNASeq</t>
   </si>
   <si>
-    <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling; 10x Genomics Chromium Next GEM Single Cell  3' Gene Expression Library Preparation v3.1  with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation</t>
+    <t>10X Genomics Next GEM Single Cell  3' Gene Expression Library prep v3.1  with UDI; 10X Genomics Sigle Cell 3' Cell Multiplexing with UDI; 10x Genomics Chromium Singel Cell Fixed RNA Profiling; 10x Genomics Chromium Next GEM Single Cell  3' Gene Expression Library Preparation v3.1  with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation with UDI; 10x Genomics Chromium GEM-X Single Cell 3' v4 Gene Expression Library Preparation; 10x Genomics Chromium Next GEM Single Cell 3' v3.1 Gene Expression Library Preparation</t>
+  </si>
+  <si>
+    <t>--config /home/tomatosrvs/AutoAnalysis/autoAnalysis.multiqc.config.yaml</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,7 +581,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -597,7 +597,7 @@
     </row>
     <row r="5" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -608,13 +608,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="7" customFormat="1" ht="136" x14ac:dyDescent="0.2">
@@ -622,13 +622,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -636,46 +636,46 @@
         <v>0</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>8</v>
@@ -684,7 +684,7 @@
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="D12" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -692,13 +692,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -706,18 +706,18 @@
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -728,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -742,13 +742,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>